<commit_message>
Install nodemon, setup list of html pages
</commit_message>
<xml_diff>
--- a/docs/Working Paper Project.xlsx
+++ b/docs/Working Paper Project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Challenge Gold\24001107-44-Nir-namaproject-ChallengeGold\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Challenge Gold\24001107-44-Nir-namaproject-ChallengeGold\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F966D8-8122-4979-99A2-AF6BF2361954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE5CB38-8477-4743-AC02-B63088431346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{30945680-93E9-4D10-B37F-7B744EE4DE2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{30945680-93E9-4D10-B37F-7B744EE4DE2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -246,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -276,7 +276,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,7 +630,7 @@
   <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +678,7 @@
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="11">
+      <c r="B6" s="1">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">

</xml_diff>

<commit_message>
Setting timeline and update Read me
</commit_message>
<xml_diff>
--- a/docs/Working Paper Project.xlsx
+++ b/docs/Working Paper Project.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Challenge Gold\24001107-44-Nir-namaproject-ChallengeGold\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864EE554-2F8D-4F22-8CB7-50E362F9CD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DB5321-1CDD-45A4-AB0D-39EB84A6753E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{30945680-93E9-4D10-B37F-7B744EE4DE2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{30945680-93E9-4D10-B37F-7B744EE4DE2D}"/>
   </bookViews>
   <sheets>
     <sheet name="CRUD" sheetId="1" r:id="rId1"/>
     <sheet name="Pages" sheetId="3" r:id="rId2"/>
+    <sheet name="Timeline" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
   <si>
     <t>CRUD</t>
   </si>
@@ -320,13 +321,67 @@
   </si>
   <si>
     <t>Terms &amp; Conditions</t>
+  </si>
+  <si>
+    <t>Days Left</t>
+  </si>
+  <si>
+    <t>Agenda</t>
+  </si>
+  <si>
+    <t>Gold Challenge Submission Due Date</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>Customer Page (My Cart, My Orders)</t>
+  </si>
+  <si>
+    <t>Product Detail Page</t>
+  </si>
+  <si>
+    <t>Login / Register Page</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Admin Page (Change Banner, Product List (Add, Delete), Order List, Change Password)</t>
+  </si>
+  <si>
+    <t>Front End</t>
+  </si>
+  <si>
+    <t>Back End</t>
+  </si>
+  <si>
+    <t>Aspect</t>
+  </si>
+  <si>
+    <t>Login and Register Process</t>
+  </si>
+  <si>
+    <t>Product List Process</t>
+  </si>
+  <si>
+    <t>Change Password Process</t>
+  </si>
+  <si>
+    <t>Check Out Process</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="ddd\,\ dd\-mmm\-yy"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +401,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -392,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -415,11 +478,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -460,6 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -478,7 +553,25 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199DB725-114C-457D-803B-1440B298B799}">
   <dimension ref="B1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="134" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D25"/>
+    <sheetView zoomScale="134" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,13 +959,13 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="22">
         <v>1</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="9" t="s">
@@ -886,9 +979,9 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="23"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="20"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="9" t="s">
         <v>22</v>
       </c>
@@ -900,9 +993,9 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="23"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="20"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="9" t="s">
         <v>26</v>
       </c>
@@ -914,9 +1007,9 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="20"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="9" t="s">
         <v>27</v>
       </c>
@@ -928,11 +1021,11 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
-      <c r="C7" s="19">
+      <c r="B7" s="24"/>
+      <c r="C7" s="20">
         <v>2</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="23" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="13" t="s">
@@ -946,9 +1039,9 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="22"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="13" t="s">
         <v>22</v>
       </c>
@@ -960,11 +1053,11 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-      <c r="C9" s="21">
+      <c r="B9" s="24"/>
+      <c r="C9" s="22">
         <v>3</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="10" t="s">
@@ -978,9 +1071,9 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="23"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="20"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="10" t="s">
         <v>22</v>
       </c>
@@ -992,9 +1085,9 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="20"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="9" t="s">
         <v>26</v>
       </c>
@@ -1006,9 +1099,9 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="20"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="9" t="s">
         <v>27</v>
       </c>
@@ -1020,11 +1113,11 @@
       </c>
     </row>
     <row r="13" spans="2:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="23"/>
-      <c r="C13" s="19">
+      <c r="B13" s="24"/>
+      <c r="C13" s="20">
         <v>4</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="23" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="13" t="s">
@@ -1038,9 +1131,9 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="22"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="13" t="s">
         <v>22</v>
       </c>
@@ -1052,9 +1145,9 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="23"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="22"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="13" t="s">
         <v>27</v>
       </c>
@@ -1066,11 +1159,11 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
-      <c r="C16" s="21">
+      <c r="B16" s="24"/>
+      <c r="C16" s="22">
         <v>5</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="21" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="9" t="s">
@@ -1084,9 +1177,9 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="23"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="20"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="9" t="s">
         <v>22</v>
       </c>
@@ -1098,9 +1191,9 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="23"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="20"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="21"/>
       <c r="E18" s="9" t="s">
         <v>26</v>
       </c>
@@ -1112,9 +1205,9 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="23"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="20"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="9" t="s">
         <v>27</v>
       </c>
@@ -1126,13 +1219,13 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="20">
         <v>1</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="23" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="13" t="s">
@@ -1146,9 +1239,9 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="22"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="13" t="s">
         <v>22</v>
       </c>
@@ -1160,9 +1253,9 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="22"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="13" t="s">
         <v>26</v>
       </c>
@@ -1174,9 +1267,9 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="22"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="13" t="s">
         <v>27</v>
       </c>
@@ -1188,11 +1281,11 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="18"/>
-      <c r="C24" s="21">
+      <c r="B24" s="19"/>
+      <c r="C24" s="22">
         <v>2</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="9" t="s">
@@ -1206,9 +1299,9 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="18"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="20"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="9" t="s">
         <v>26</v>
       </c>
@@ -1247,7 +1340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9115E4-A012-4C5A-BC6F-EBC7ABD14DDB}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1433,7 +1526,7 @@
       <c r="A18" s="7">
         <v>14</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="18" t="s">
         <v>81</v>
       </c>
       <c r="C18" s="15"/>
@@ -1502,4 +1595,239 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330AA3CD-A9E9-4B69-9E63-F60DA61ED8D5}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="25">
+        <f ca="1">TODAY()</f>
+        <v>45401</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="28">
+        <v>1</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="29">
+        <v>45403</v>
+      </c>
+      <c r="E3" s="28">
+        <f ca="1">D3-$G$1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="28">
+        <v>2</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="29">
+        <v>45403</v>
+      </c>
+      <c r="E4" s="28">
+        <f ca="1">D4-$G$1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="28">
+        <v>3</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="29">
+        <f>D4+4</f>
+        <v>45407</v>
+      </c>
+      <c r="E5" s="28">
+        <f ca="1">D5-$G$1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
+        <v>4</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="29">
+        <f>D5+10</f>
+        <v>45417</v>
+      </c>
+      <c r="E6" s="28">
+        <f ca="1">D6-$G$1</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="28">
+        <v>5</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="29">
+        <f>D6+5</f>
+        <v>45422</v>
+      </c>
+      <c r="E7" s="28">
+        <f ca="1">D7-$G$1</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="28">
+        <v>6</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="29">
+        <f>D7+10</f>
+        <v>45432</v>
+      </c>
+      <c r="E8" s="28">
+        <f ca="1">D8-$G$1</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
+        <v>7</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="29">
+        <f>D8+2</f>
+        <v>45434</v>
+      </c>
+      <c r="E9" s="28">
+        <f ca="1">D9-$G$1</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="28">
+        <v>8</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="29">
+        <f>D9+10</f>
+        <v>45444</v>
+      </c>
+      <c r="E10" s="28">
+        <f ca="1">D10-$G$1</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="28">
+        <v>9</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="29">
+        <f>D10+10</f>
+        <v>45454</v>
+      </c>
+      <c r="E11" s="28">
+        <f ca="1">D11-$G$1</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="28">
+        <v>12</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="29">
+        <v>45446</v>
+      </c>
+      <c r="E12" s="28">
+        <f ca="1">D12-$G$1</f>
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
May 14, 2024, 8:12 PM
</commit_message>
<xml_diff>
--- a/docs/Working Paper Project.xlsx
+++ b/docs/Working Paper Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Challenge Gold\24001107-44-Nir-namaproject-ChallengeGold\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DB5321-1CDD-45A4-AB0D-39EB84A6753E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6597212-ACBA-432D-A667-AFCE690ECC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{30945680-93E9-4D10-B37F-7B744EE4DE2D}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{30945680-93E9-4D10-B37F-7B744EE4DE2D}"/>
   </bookViews>
   <sheets>
     <sheet name="CRUD" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
   <si>
     <t>CRUD</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -379,7 +382,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="ddd\,\ dd\-mmm\-yy"/>
+    <numFmt numFmtId="164" formatCode="ddd\,\ dd\-mmm\-yy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -493,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -535,24 +538,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -563,14 +548,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -959,13 +965,13 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="29">
         <v>1</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="28" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="9" t="s">
@@ -979,9 +985,9 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="21"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="9" t="s">
         <v>22</v>
       </c>
@@ -993,9 +999,9 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="24"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="9" t="s">
         <v>26</v>
       </c>
@@ -1007,9 +1013,9 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="24"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="21"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="9" t="s">
         <v>27</v>
       </c>
@@ -1021,11 +1027,11 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="24"/>
-      <c r="C7" s="20">
+      <c r="B7" s="31"/>
+      <c r="C7" s="27">
         <v>2</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="30" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="13" t="s">
@@ -1039,9 +1045,9 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="24"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="13" t="s">
         <v>22</v>
       </c>
@@ -1053,11 +1059,11 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="24"/>
-      <c r="C9" s="22">
+      <c r="B9" s="31"/>
+      <c r="C9" s="29">
         <v>3</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="28" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="10" t="s">
@@ -1071,9 +1077,9 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="24"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="21"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="10" t="s">
         <v>22</v>
       </c>
@@ -1085,9 +1091,9 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="24"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="9" t="s">
         <v>26</v>
       </c>
@@ -1099,9 +1105,9 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="21"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="9" t="s">
         <v>27</v>
       </c>
@@ -1113,11 +1119,11 @@
       </c>
     </row>
     <row r="13" spans="2:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="24"/>
-      <c r="C13" s="20">
+      <c r="B13" s="31"/>
+      <c r="C13" s="27">
         <v>4</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="30" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="13" t="s">
@@ -1131,9 +1137,9 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="13" t="s">
         <v>22</v>
       </c>
@@ -1145,9 +1151,9 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="24"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="13" t="s">
         <v>27</v>
       </c>
@@ -1159,11 +1165,11 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="24"/>
-      <c r="C16" s="22">
+      <c r="B16" s="31"/>
+      <c r="C16" s="29">
         <v>5</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="28" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="9" t="s">
@@ -1177,9 +1183,9 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="24"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="21"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="28"/>
       <c r="E17" s="9" t="s">
         <v>22</v>
       </c>
@@ -1191,9 +1197,9 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="24"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="21"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="28"/>
       <c r="E18" s="9" t="s">
         <v>26</v>
       </c>
@@ -1205,9 +1211,9 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="24"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="9" t="s">
         <v>27</v>
       </c>
@@ -1219,13 +1225,13 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="27">
         <v>1</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="30" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="13" t="s">
@@ -1239,9 +1245,9 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="23"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="13" t="s">
         <v>22</v>
       </c>
@@ -1253,9 +1259,9 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="23"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="30"/>
       <c r="E22" s="13" t="s">
         <v>26</v>
       </c>
@@ -1267,9 +1273,9 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="23"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="13" t="s">
         <v>27</v>
       </c>
@@ -1281,11 +1287,11 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="22">
+      <c r="B24" s="26"/>
+      <c r="C24" s="29">
         <v>2</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="28" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="9" t="s">
@@ -1299,9 +1305,9 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="9" t="s">
         <v>26</v>
       </c>
@@ -1602,7 +1608,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E5" sqref="E5:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,213 +1623,205 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G1" s="25">
+      <c r="G1" s="19">
         <f ca="1">TODAY()</f>
-        <v>45401</v>
+        <v>45425</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="20" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="28">
+      <c r="A3" s="22">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="29">
-        <v>45403</v>
-      </c>
-      <c r="E3" s="28">
-        <f ca="1">D3-$G$1</f>
+      <c r="D3" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
+      <c r="B4" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="22">
+        <v>3</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="23">
+        <v>45427</v>
+      </c>
+      <c r="E5" s="22">
+        <f t="shared" ref="E3:E12" ca="1" si="0">D5-$G$1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="27" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="22">
+        <v>4</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="29">
-        <v>45403</v>
-      </c>
-      <c r="E4" s="28">
-        <f ca="1">D4-$G$1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
-        <v>3</v>
-      </c>
-      <c r="B5" s="27" t="s">
+      <c r="C6" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="23">
+        <f>D5+2</f>
+        <v>45429</v>
+      </c>
+      <c r="E6" s="22">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
+        <v>5</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="29">
-        <f>D4+4</f>
-        <v>45407</v>
-      </c>
-      <c r="E5" s="28">
-        <f ca="1">D5-$G$1</f>
+      <c r="C7" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="23">
+        <f>D6</f>
+        <v>45429</v>
+      </c>
+      <c r="E7" s="22">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="28">
-        <v>4</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="29">
-        <f>D5+10</f>
-        <v>45417</v>
-      </c>
-      <c r="E6" s="28">
-        <f ca="1">D6-$G$1</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
-        <v>5</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="29">
-        <f>D6+5</f>
-        <v>45422</v>
-      </c>
-      <c r="E7" s="28">
-        <f ca="1">D7-$G$1</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="28">
+      <c r="B8" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="23">
+        <v>45431</v>
+      </c>
+      <c r="E8" s="22">
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="27" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>7</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="29">
-        <f>D7+10</f>
-        <v>45432</v>
-      </c>
-      <c r="E8" s="28">
-        <f ca="1">D8-$G$1</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
-        <v>7</v>
-      </c>
-      <c r="B9" s="27" t="s">
+      <c r="C9" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="23">
+        <f>D8</f>
+        <v>45431</v>
+      </c>
+      <c r="E9" s="22">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="22">
+        <v>8</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="29">
-        <f>D8+2</f>
-        <v>45434</v>
-      </c>
-      <c r="E9" s="28">
-        <f ca="1">D9-$G$1</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="28">
-        <v>8</v>
-      </c>
-      <c r="B10" s="27" t="s">
+      <c r="C10" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="23">
+        <f>D9+5</f>
+        <v>45436</v>
+      </c>
+      <c r="E10" s="22">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="22">
+        <v>9</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="29">
-        <f>D9+10</f>
-        <v>45444</v>
-      </c>
-      <c r="E10" s="28">
-        <f ca="1">D10-$G$1</f>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
-        <v>9</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="29">
-        <f>D10+10</f>
-        <v>45454</v>
-      </c>
-      <c r="E11" s="28">
-        <f ca="1">D11-$G$1</f>
-        <v>53</v>
+      <c r="D11" s="23">
+        <f>D10+3</f>
+        <v>45439</v>
+      </c>
+      <c r="E11" s="22">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="28">
+      <c r="A12" s="22">
         <v>12</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="29">
-        <v>45446</v>
-      </c>
-      <c r="E12" s="28">
-        <f ca="1">D12-$G$1</f>
-        <v>45</v>
+      <c r="D12" s="23">
+        <v>45445</v>
+      </c>
+      <c r="E12" s="22">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
May 18, 2024, 9:47 AM
</commit_message>
<xml_diff>
--- a/docs/Working Paper Project.xlsx
+++ b/docs/Working Paper Project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Challenge Gold\24001107-44-Nir-namaproject-ChallengeGold\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6597212-ACBA-432D-A667-AFCE690ECC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE2081F-FE9E-4191-AA89-0A0B0D61DD51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{30945680-93E9-4D10-B37F-7B744EE4DE2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{30945680-93E9-4D10-B37F-7B744EE4DE2D}"/>
   </bookViews>
   <sheets>
     <sheet name="CRUD" sheetId="1" r:id="rId1"/>
@@ -557,6 +557,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -573,9 +576,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -965,13 +965,13 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="30">
         <v>1</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="9" t="s">
@@ -985,9 +985,9 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="31"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="28"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="9" t="s">
         <v>22</v>
       </c>
@@ -999,9 +999,9 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="31"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="28"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="9" t="s">
         <v>26</v>
       </c>
@@ -1013,9 +1013,9 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="31"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="28"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="9" t="s">
         <v>27</v>
       </c>
@@ -1027,11 +1027,11 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
-      <c r="C7" s="27">
+      <c r="B7" s="32"/>
+      <c r="C7" s="28">
         <v>2</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="31" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="13" t="s">
@@ -1045,9 +1045,9 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="31"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="30"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="13" t="s">
         <v>22</v>
       </c>
@@ -1059,11 +1059,11 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="31"/>
-      <c r="C9" s="29">
+      <c r="B9" s="32"/>
+      <c r="C9" s="30">
         <v>3</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="29" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="10" t="s">
@@ -1077,9 +1077,9 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="31"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="28"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="10" t="s">
         <v>22</v>
       </c>
@@ -1091,9 +1091,9 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="28"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="9" t="s">
         <v>26</v>
       </c>
@@ -1105,9 +1105,9 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="31"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="28"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="9" t="s">
         <v>27</v>
       </c>
@@ -1119,11 +1119,11 @@
       </c>
     </row>
     <row r="13" spans="2:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="31"/>
-      <c r="C13" s="27">
+      <c r="B13" s="32"/>
+      <c r="C13" s="28">
         <v>4</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="31" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="13" t="s">
@@ -1137,9 +1137,9 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="31"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="30"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="31"/>
       <c r="E14" s="13" t="s">
         <v>22</v>
       </c>
@@ -1151,9 +1151,9 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="31"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="30"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="13" t="s">
         <v>27</v>
       </c>
@@ -1165,11 +1165,11 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="31"/>
-      <c r="C16" s="29">
+      <c r="B16" s="32"/>
+      <c r="C16" s="30">
         <v>5</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="29" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="9" t="s">
@@ -1183,9 +1183,9 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="31"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="28"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="9" t="s">
         <v>22</v>
       </c>
@@ -1197,9 +1197,9 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="31"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="28"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="9" t="s">
         <v>26</v>
       </c>
@@ -1211,9 +1211,9 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="31"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="28"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="9" t="s">
         <v>27</v>
       </c>
@@ -1225,13 +1225,13 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="28">
         <v>1</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="13" t="s">
@@ -1245,9 +1245,9 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="26"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="30"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="13" t="s">
         <v>22</v>
       </c>
@@ -1259,9 +1259,9 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="26"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="30"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="13" t="s">
         <v>26</v>
       </c>
@@ -1273,9 +1273,9 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="26"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="30"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="13" t="s">
         <v>27</v>
       </c>
@@ -1287,11 +1287,11 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="26"/>
-      <c r="C24" s="29">
+      <c r="B24" s="27"/>
+      <c r="C24" s="30">
         <v>2</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="29" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="9" t="s">
@@ -1305,9 +1305,9 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="26"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="28"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="9" t="s">
         <v>26</v>
       </c>
@@ -1608,7 +1608,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,7 +1625,7 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1" s="19">
         <f ca="1">TODAY()</f>
-        <v>45425</v>
+        <v>45429</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1655,7 +1655,7 @@
       <c r="C3" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="26" t="s">
         <v>108</v>
       </c>
       <c r="E3" s="22"/>
@@ -1670,7 +1670,7 @@
       <c r="C4" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="26" t="s">
         <v>108</v>
       </c>
       <c r="E4" s="22"/>
@@ -1689,8 +1689,8 @@
         <v>45427</v>
       </c>
       <c r="E5" s="22">
-        <f t="shared" ref="E3:E12" ca="1" si="0">D5-$G$1</f>
-        <v>2</v>
+        <f t="shared" ref="E5:E12" ca="1" si="0">D5-$G$1</f>
+        <v>-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="E6" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1728,7 +1728,7 @@
       </c>
       <c r="E7" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="E8" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="E9" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="E10" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="E11" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="E12" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
May 31, 2024, 4:12 PM
</commit_message>
<xml_diff>
--- a/docs/Working Paper Project.xlsx
+++ b/docs/Working Paper Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Challenge Gold\24001107-44-Nir-namaproject-ChallengeGold\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14016AF0-377D-45B7-BECE-E2C50F379944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DD3A6B-72BE-4456-B951-E2CBBE079FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{30945680-93E9-4D10-B37F-7B744EE4DE2D}"/>
   </bookViews>
@@ -1807,7 +1807,7 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1" s="19">
         <f ca="1">TODAY()</f>
-        <v>45442</v>
+        <v>45443</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1872,7 +1872,7 @@
       </c>
       <c r="E5" s="22">
         <f t="shared" ref="E5:E12" ca="1" si="0">D5-$G$1</f>
-        <v>-15</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="E6" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>-13</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="E7" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>-13</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1928,7 +1928,7 @@
       </c>
       <c r="E8" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>-11</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="E9" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>-11</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="E10" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>-6</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="E11" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="E12" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2017,7 +2017,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Jun 1, 2024, 11:06 AM
</commit_message>
<xml_diff>
--- a/docs/Working Paper Project.xlsx
+++ b/docs/Working Paper Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Challenge Gold\24001107-44-Nir-namaproject-ChallengeGold\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DD3A6B-72BE-4456-B951-E2CBBE079FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB748CBB-1146-4082-975E-FE8141662E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{30945680-93E9-4D10-B37F-7B744EE4DE2D}"/>
+    <workbookView xWindow="-4830" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{30945680-93E9-4D10-B37F-7B744EE4DE2D}"/>
   </bookViews>
   <sheets>
     <sheet name="CRUD" sheetId="1" r:id="rId1"/>
@@ -1807,7 +1807,7 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1" s="19">
         <f ca="1">TODAY()</f>
-        <v>45443</v>
+        <v>45444</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1872,7 +1872,7 @@
       </c>
       <c r="E5" s="22">
         <f t="shared" ref="E5:E12" ca="1" si="0">D5-$G$1</f>
-        <v>-16</v>
+        <v>-17</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="E6" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>-14</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="E7" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>-14</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1928,7 +1928,7 @@
       </c>
       <c r="E8" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>-12</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="E9" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>-12</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="E10" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="E11" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>-4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="E12" s="22">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2017,7 +2017,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>